<commit_message>
Another day of learning
</commit_message>
<xml_diff>
--- a/Financial Modelling with Nick DeRobertis/Basic Retirement Model/Basic Retirement Model.xlsx
+++ b/Financial Modelling with Nick DeRobertis/Basic Retirement Model/Basic Retirement Model.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\WeeKe\Desktop\Learning\Financial Modelling with Nick DeRobertis\Basic Retirement Model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16E6D81A-4F6D-4D19-8328-A8976DF07B32}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D0B20D7-06B5-4403-BD99-596C01F294DA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="41610" yWindow="1275" windowWidth="21600" windowHeight="9945" activeTab="2" xr2:uid="{7A004675-3EAC-41CA-8ED1-983310818834}"/>
+    <workbookView xWindow="36000" yWindow="1275" windowWidth="17280" windowHeight="7950" activeTab="2" xr2:uid="{7A004675-3EAC-41CA-8ED1-983310818834}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="13">
   <si>
     <t>Inputs</t>
   </si>
@@ -66,6 +66,15 @@
   </si>
   <si>
     <t>Savings Rate</t>
+  </si>
+  <si>
+    <t>Determining salary at any given year</t>
+  </si>
+  <si>
+    <t>Determining wealth of an individual after he saves</t>
+  </si>
+  <si>
+    <t>Determining years to retirement based on individual's wealth</t>
   </si>
 </sst>
 </file>
@@ -157,15 +166,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -495,63 +504,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
+      <c r="B1" s="9"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="4">
+      <c r="B2" s="3">
         <v>10000</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="5">
+      <c r="B3" s="4">
         <v>0.25</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="5">
+      <c r="B4" s="4">
         <v>0.05</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="6">
+      <c r="B5" s="5">
         <v>1500000</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="3"/>
+      <c r="B7" s="9"/>
     </row>
     <row r="8" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="4">
+      <c r="B8" s="3">
         <f>B2*B3</f>
         <v>2500</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="4">
+      <c r="B9" s="3">
         <f>NPER(B4,-B8,0,B5)</f>
         <v>70.382776179232522</v>
       </c>
@@ -580,32 +589,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
+      <c r="B1" s="9"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="4">
+      <c r="B2" s="3">
         <v>10000</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="5">
+      <c r="B3" s="4">
         <v>0.25</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="5">
+      <c r="B4" s="4">
         <v>0.05</v>
       </c>
       <c r="C4" s="1">
@@ -616,41 +625,41 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="6">
+      <c r="B5" s="5">
         <v>1500000</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="3"/>
+      <c r="B7" s="9"/>
     </row>
     <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="4">
+      <c r="B8" s="3">
         <f>B2*B3</f>
         <v>2500</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="4">
+      <c r="B9" s="3">
         <f>NPER(B4,-$B$8,0,$B$5)</f>
         <v>70.382776179232522</v>
       </c>
-      <c r="C9" s="4">
+      <c r="C9" s="3">
         <f>NPER(C4,-$B$8,0,$B$5)</f>
         <v>61.969891472163098</v>
       </c>
-      <c r="D9" s="4">
+      <c r="D9" s="3">
         <f>NPER(D4,-$B$8,0,$B$5)</f>
         <v>55.590825423437416</v>
       </c>
@@ -666,10 +675,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A16254F-F394-425E-B148-937E5AB59855}">
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="A22" sqref="A22:A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -679,56 +688,56 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
+      <c r="B1" s="9"/>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="4">
+      <c r="B2" s="3">
         <v>10000</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="9">
+      <c r="B3" s="8">
         <v>0.1</v>
       </c>
-      <c r="C3" s="5">
+      <c r="C3" s="4">
         <v>0.25</v>
       </c>
-      <c r="D3" s="5">
+      <c r="D3" s="4">
         <v>0.4</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="9">
+      <c r="B4" s="8">
         <v>0.05</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C4" s="4">
         <v>0.06</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4" s="4">
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="8">
+      <c r="B5" s="7">
         <v>1500000</v>
       </c>
       <c r="C5" s="2"/>
@@ -741,43 +750,43 @@
       <c r="D6" s="2"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="3"/>
+      <c r="B7" s="9"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
     </row>
     <row r="8" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="4">
+      <c r="B8" s="3">
         <f>$B$2*B3</f>
         <v>1000</v>
       </c>
-      <c r="C8" s="4">
+      <c r="C8" s="3">
         <f>$B$2*C3</f>
         <v>2500</v>
       </c>
-      <c r="D8" s="4">
-        <f t="shared" ref="C8:D8" si="0">$B$2*D3</f>
+      <c r="D8" s="3">
+        <f t="shared" ref="D8" si="0">$B$2*D3</f>
         <v>4000</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="4">
+      <c r="B9" s="3">
         <f>NPER(B4,-$B$8,0,$B$5)</f>
         <v>88.762426075205056</v>
       </c>
-      <c r="C9" s="4">
+      <c r="C9" s="3">
         <f>NPER(C4,-$B$8,0,$B$5)</f>
         <v>77.414519196400946</v>
       </c>
-      <c r="D9" s="4">
+      <c r="D9" s="3">
         <f>NPER(D4,-$B$8,0,$B$5)</f>
         <v>68.925986541349602</v>
       </c>
@@ -785,79 +794,94 @@
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
-      <c r="C14" s="5">
+      <c r="C14" s="4">
         <v>0.05</v>
       </c>
-      <c r="D14" s="5">
+      <c r="D14" s="4">
         <v>0.06</v>
       </c>
-      <c r="E14" s="5">
+      <c r="E14" s="4">
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" s="3" t="s">
+      <c r="A15" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B15" s="5">
+      <c r="B15" s="4">
         <v>0.1</v>
       </c>
-      <c r="C15" s="4">
+      <c r="C15" s="3">
         <f>NPER(C14,-$B$8,0,$B$5)</f>
         <v>88.762426075205056</v>
       </c>
-      <c r="D15" s="4">
+      <c r="D15" s="3">
         <f>NPER(D14,-$B$8,0,$B$5)</f>
         <v>77.414519196400946</v>
       </c>
-      <c r="E15" s="4">
+      <c r="E15" s="3">
         <f>NPER(E14,-$B$8,0,$B$5)</f>
         <v>68.925986541349602</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" s="3"/>
-      <c r="B16" s="5">
+      <c r="A16" s="9"/>
+      <c r="B16" s="4">
         <v>0.25</v>
       </c>
-      <c r="C16" s="4">
+      <c r="C16" s="3">
         <f>NPER(C14,-$C$8,0,$B$5)</f>
         <v>70.382776179232522</v>
       </c>
-      <c r="D16" s="4">
+      <c r="D16" s="3">
         <f>NPER(D14,-$C$8,0,$B$5)</f>
         <v>61.969891472163098</v>
       </c>
-      <c r="E16" s="4">
-        <f t="shared" ref="D16:E16" si="1">NPER(E14,-$C$8,0,$B$5)</f>
+      <c r="E16" s="3">
+        <f t="shared" ref="E16" si="1">NPER(E14,-$C$8,0,$B$5)</f>
         <v>55.590825423437416</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" s="3"/>
-      <c r="B17" s="5">
+      <c r="A17" s="9"/>
+      <c r="B17" s="4">
         <v>0.4</v>
       </c>
-      <c r="C17" s="4">
+      <c r="C17" s="3">
         <f>NPER(C14,-$D$8,0,$B$5)</f>
         <v>61.142518008089269</v>
       </c>
-      <c r="D17" s="4">
+      <c r="D17" s="3">
         <f t="shared" ref="D17:E17" si="2">NPER(D14,-$D$8,0,$B$5)</f>
         <v>54.179845183182813</v>
       </c>
-      <c r="E17" s="4">
+      <c r="E17" s="3">
         <f t="shared" si="2"/>
         <v>48.848943862488909</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>